<commit_message>
update backend code for Date Formatting[mm/dd/yyyy]
</commit_message>
<xml_diff>
--- a/backend/uploads/Projects_Complex.xlsx
+++ b/backend/uploads/Projects_Complex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R.Sanjay\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C32453B-4D97-47BC-93AF-20E03C2D12FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7A6391-0379-4532-9E7B-3BED24B11F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,9 +476,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>